<commit_message>
Calculation table for Levenshtein edit distance
</commit_message>
<xml_diff>
--- a/lab8/levenshtein_Calc.xlsx
+++ b/lab8/levenshtein_Calc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
   <si>
     <t>l</t>
   </si>
@@ -42,15 +42,6 @@
   </si>
   <si>
     <t>j</t>
-  </si>
-  <si>
-    <t>- d[i-1,j]+1</t>
-  </si>
-  <si>
-    <t>- d[i,j-1]+1</t>
-  </si>
-  <si>
-    <t>- d[i-1,j-1]+cost[i,j]</t>
   </si>
   <si>
     <t>g</t>
@@ -386,10 +377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="169" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -399,7 +390,7 @@
     <col min="11" max="12" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C1">
         <v>1</v>
       </c>
@@ -422,7 +413,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -442,7 +433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -468,7 +459,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -503,7 +494,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -538,7 +529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -573,7 +564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -608,7 +599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -643,7 +634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -678,7 +669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -713,50 +704,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="M14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="M15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="M16" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" t="s">
         <v>8</v>
       </c>
-      <c r="E18" t="s">
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" t="s">
         <v>9</v>
       </c>
-      <c r="F18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" t="s">
-        <v>12</v>
-      </c>
       <c r="J18" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L18" t="s">
         <v>0</v>
@@ -796,34 +772,178 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>MIN(D19+1,C20+1,C19+(IF(D$18=$B20,0,1)))</f>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20:L28" si="7">MIN(E19+1,D20+1,D19+(IF(E$18=$B20,0,1)))</f>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="7"/>
         <v>8</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D28" si="8">MIN(D20+1,C21+1,C20+(IF(D$18=$B21,0,1)))</f>
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C22">
         <v>3</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="7"/>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>4</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="7"/>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
@@ -833,22 +953,130 @@
       <c r="C24">
         <v>5</v>
       </c>
+      <c r="D24">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C25">
         <v>6</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <v>7</v>
       </c>
+      <c r="D26">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
@@ -857,6 +1085,42 @@
       <c r="C27">
         <v>8</v>
       </c>
+      <c r="D27">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
@@ -864,6 +1128,42 @@
       </c>
       <c r="C28">
         <v>9</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="7"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>